<commit_message>
ResourceMonitor v1.1.2 code refactoring / Readme v0.0.2 usage menu, image updated
</commit_message>
<xml_diff>
--- a/문제.xlsx
+++ b/문제.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9108" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9108" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="기타문제" sheetId="2" r:id="rId1"/>
@@ -646,47 +646,123 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>300517</xdr:colOff>
+      <xdr:colOff>176675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>74336</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="220980"/>
+          <a:ext cx="10136015" cy="295316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>486858</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>181000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="662940"/>
+          <a:ext cx="7763958" cy="181000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>395780</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="그림 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="220980"/>
-          <a:ext cx="10259857" cy="295316"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1104900"/>
+          <a:ext cx="10355120" cy="342948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>363016</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>219106</xdr:rowOff>
+      <xdr:colOff>324911</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190527</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -696,15 +772,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="662940"/>
-          <a:ext cx="7640116" cy="219106"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1546860"/>
+          <a:ext cx="7602011" cy="190527"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1037,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K9:K10"/>
     </sheetView>
   </sheetViews>
@@ -1061,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1074,7 +1150,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="2">
-        <v>44510.75277777778</v>
+        <v>44511.615972222222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2">
+        <v>44511.75277777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>